<commit_message>
prices, tech: added second (promo) price to the [price] document.
</commit_message>
<xml_diff>
--- a/htdocs/assets/prices.xlsx
+++ b/htdocs/assets/prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -73,10 +73,16 @@
     <t xml:space="preserve">Название продукта</t>
   </si>
   <si>
-    <t xml:space="preserve">Цена на полке</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПРОМО</t>
+    <t xml:space="preserve">Регулярная цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРОМО цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Скидка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гранул. продукта</t>
   </si>
   <si>
     <t xml:space="preserve">РРЦ</t>
@@ -94,10 +100,10 @@
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0"/>
@@ -225,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,6 +322,10 @@
     </xf>
     <xf numFmtId="168" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -391,18 +401,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,16 +433,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="34.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="5" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="7.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="5" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="4.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="63" min="23" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="64" style="8" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="5" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="5" width="11.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="4.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="25" style="7" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="66" style="8" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="11"/>
@@ -450,10 +461,11 @@
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
       <c r="R1" s="12"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="11"/>
-      <c r="AMJ1" s="0"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
@@ -510,17 +522,23 @@
       <c r="R2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="17" t="s">
         <v>21</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -570,31 +588,40 @@
         <v>15</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="R3" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="S3" s="22" t="n">
+      <c r="S3" s="21" t="n">
         <v>19</v>
       </c>
-      <c r="T3" s="21" t="n">
+      <c r="T3" s="22" t="n">
         <v>20</v>
       </c>
-      <c r="U3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="U3" s="22" t="n">
+        <v>21</v>
+      </c>
+      <c r="V3" s="21" t="n">
+        <v>22</v>
+      </c>
+      <c r="W3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W4" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
price, tech: added [note] ant [photo] attribute to the [price] document.
</commit_message>
<xml_diff>
--- a/htdocs/assets/prices.xlsx
+++ b/htdocs/assets/prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -88,6 +88,12 @@
     <t xml:space="preserve">РРЦ</t>
   </si>
   <si>
+    <t xml:space="preserve">Фото</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Примечание</t>
+  </si>
+  <si>
     <t xml:space="preserve">Руководитель</t>
   </si>
   <si>
@@ -104,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
   </si>
 </sst>
 </file>
@@ -224,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,10 +307,6 @@
     </xf>
     <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -378,14 +386,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1048576"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -410,10 +418,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="7.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="11.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="5" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="3" width="19.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="4.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="65" min="25" style="7" width="8.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="66" style="8" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="27.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="3" width="19.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="4.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="67" min="27" style="7" width="8.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="68" style="8" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -486,8 +496,14 @@
       <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -537,10 +553,10 @@
         <v>15</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R2" s="16" t="n">
         <v>18</v>
@@ -558,16 +574,18 @@
         <v>22</v>
       </c>
       <c r="W2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W3" s="18"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>